<commit_message>
updated the validationMain and the way analytic results are obtained
1. Changed the query source from IHPC to Postgres
2. Added/modified some data process procedures based on the exact data
from Postgres
3. Added the feedback of am_track, pm_track and durations
4. added some testing results "testRestul1.txt" and"testRestul2.txt" for
reference
</commit_message>
<xml_diff>
--- a/nodes for testing auto-validation.xlsx
+++ b/nodes for testing auto-validation.xlsx
@@ -1012,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1030,23 +1030,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>400040</v>
+        <v>509057</v>
       </c>
       <c r="B2">
-        <v>20151104</v>
+        <v>20150930</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>509052</v>
+        <v>509057</v>
       </c>
       <c r="B3">
-        <v>20150929</v>
+        <v>20151001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>509052</v>
+        <v>509059</v>
       </c>
       <c r="B4">
         <v>20150930</v>
@@ -1054,23 +1054,23 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>509057</v>
+        <v>509059</v>
       </c>
       <c r="B5">
-        <v>20150930</v>
+        <v>20151001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>509057</v>
+        <v>512116</v>
       </c>
       <c r="B6">
-        <v>20151001</v>
+        <v>20150929</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>509059</v>
+        <v>512117</v>
       </c>
       <c r="B7">
         <v>20150930</v>
@@ -1078,31 +1078,31 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>509059</v>
+        <v>512118</v>
       </c>
       <c r="B8">
-        <v>20151001</v>
+        <v>20150930</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>512116</v>
+        <v>512118</v>
       </c>
       <c r="B9">
-        <v>20150929</v>
+        <v>20151001</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>512117</v>
+        <v>512119</v>
       </c>
       <c r="B10">
-        <v>20150930</v>
+        <v>20150929</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>512118</v>
+        <v>512119</v>
       </c>
       <c r="B11">
         <v>20150930</v>
@@ -1110,31 +1110,31 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>512118</v>
+        <v>512123</v>
       </c>
       <c r="B12">
-        <v>20151001</v>
+        <v>20150930</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>512119</v>
+        <v>512123</v>
       </c>
       <c r="B13">
-        <v>20150929</v>
+        <v>20151001</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>512119</v>
+        <v>512124</v>
       </c>
       <c r="B14">
-        <v>20150930</v>
+        <v>20150929</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>512123</v>
+        <v>512124</v>
       </c>
       <c r="B15">
         <v>20150930</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>512123</v>
+        <v>512124</v>
       </c>
       <c r="B16">
         <v>20151001</v>
@@ -1150,7 +1150,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>512124</v>
+        <v>513425</v>
       </c>
       <c r="B17">
         <v>20150929</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>512124</v>
+        <v>513425</v>
       </c>
       <c r="B18">
         <v>20150930</v>
@@ -1166,7 +1166,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>512124</v>
+        <v>513425</v>
       </c>
       <c r="B19">
         <v>20151001</v>
@@ -1174,15 +1174,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>513425</v>
+        <v>513427</v>
       </c>
       <c r="B20">
-        <v>20150929</v>
+        <v>20150930</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>513425</v>
+        <v>513432</v>
       </c>
       <c r="B21">
         <v>20150930</v>
@@ -1190,15 +1190,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>513425</v>
+        <v>513435</v>
       </c>
       <c r="B22">
-        <v>20151001</v>
+        <v>20150929</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>513427</v>
+        <v>513435</v>
       </c>
       <c r="B23">
         <v>20150930</v>
@@ -1206,15 +1206,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>513432</v>
+        <v>513435</v>
       </c>
       <c r="B24">
-        <v>20150930</v>
+        <v>20151001</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>513435</v>
+        <v>513437</v>
       </c>
       <c r="B25">
         <v>20150929</v>
@@ -1222,79 +1222,79 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>513435</v>
+        <v>513471</v>
       </c>
       <c r="B26">
-        <v>20150930</v>
+        <v>20150929</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>513435</v>
+        <v>513471</v>
       </c>
       <c r="B27">
-        <v>20151001</v>
+        <v>20150930</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>513437</v>
+        <v>513471</v>
       </c>
       <c r="B28">
-        <v>20150929</v>
+        <v>20151001</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>513471</v>
+        <v>513472</v>
       </c>
       <c r="B29">
-        <v>20150929</v>
+        <v>20150930</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>513471</v>
+        <v>513473</v>
       </c>
       <c r="B30">
-        <v>20150930</v>
+        <v>20150929</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>513471</v>
+        <v>513473</v>
       </c>
       <c r="B31">
-        <v>20151001</v>
+        <v>20150930</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>513472</v>
+        <v>513475</v>
       </c>
       <c r="B32">
-        <v>20150930</v>
+        <v>20150929</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>513473</v>
+        <v>513475</v>
       </c>
       <c r="B33">
-        <v>20150929</v>
+        <v>20150930</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>513473</v>
+        <v>513475</v>
       </c>
       <c r="B34">
-        <v>20150930</v>
+        <v>20151001</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>513475</v>
+        <v>513476</v>
       </c>
       <c r="B35">
         <v>20150929</v>
@@ -1302,7 +1302,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>513475</v>
+        <v>513476</v>
       </c>
       <c r="B36">
         <v>20150930</v>
@@ -1310,15 +1310,15 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>513475</v>
+        <v>513478</v>
       </c>
       <c r="B37">
-        <v>20151001</v>
+        <v>20150929</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>513476</v>
+        <v>514500</v>
       </c>
       <c r="B38">
         <v>20150929</v>
@@ -1326,7 +1326,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>513476</v>
+        <v>514500</v>
       </c>
       <c r="B39">
         <v>20150930</v>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>513478</v>
+        <v>514501</v>
       </c>
       <c r="B40">
         <v>20150929</v>
@@ -1342,7 +1342,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>514500</v>
+        <v>514503</v>
       </c>
       <c r="B41">
         <v>20150929</v>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>514500</v>
+        <v>514503</v>
       </c>
       <c r="B42">
         <v>20150930</v>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>514501</v>
+        <v>514505</v>
       </c>
       <c r="B43">
         <v>20150929</v>
@@ -1366,50 +1366,50 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>514503</v>
+        <v>514505</v>
       </c>
       <c r="B44">
-        <v>20150929</v>
+        <v>20150930</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>514503</v>
+        <v>514511</v>
       </c>
       <c r="B45">
-        <v>20150930</v>
+        <v>20151001</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>514505</v>
+        <v>514511</v>
       </c>
       <c r="B46">
-        <v>20150929</v>
+        <v>20151002</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>514505</v>
+        <v>514594</v>
       </c>
       <c r="B47">
-        <v>20150930</v>
+        <v>20150929</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>514511</v>
+        <v>514594</v>
       </c>
       <c r="B48">
-        <v>20151001</v>
+        <v>20150930</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>514511</v>
+        <v>514594</v>
       </c>
       <c r="B49">
-        <v>20151002</v>
+        <v>20151001</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1417,52 +1417,52 @@
         <v>514594</v>
       </c>
       <c r="B50">
-        <v>20150929</v>
+        <v>20151002</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>514594</v>
+        <v>514595</v>
       </c>
       <c r="B51">
-        <v>20150930</v>
+        <v>20150929</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>514594</v>
+        <v>514595</v>
       </c>
       <c r="B52">
-        <v>20151001</v>
+        <v>20151002</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>514594</v>
+        <v>514596</v>
       </c>
       <c r="B53">
-        <v>20151002</v>
+        <v>20150929</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>514595</v>
+        <v>514598</v>
       </c>
       <c r="B54">
-        <v>20150929</v>
+        <v>20150930</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>514595</v>
+        <v>517606</v>
       </c>
       <c r="B55">
-        <v>20151002</v>
+        <v>20150929</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>514596</v>
+        <v>517610</v>
       </c>
       <c r="B56">
         <v>20150929</v>
@@ -1470,23 +1470,23 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>514598</v>
+        <v>517612</v>
       </c>
       <c r="B57">
-        <v>20150930</v>
+        <v>20150929</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>517606</v>
+        <v>517612</v>
       </c>
       <c r="B58">
-        <v>20150929</v>
+        <v>20151002</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>517610</v>
+        <v>517617</v>
       </c>
       <c r="B59">
         <v>20150929</v>
@@ -1494,41 +1494,17 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>517612</v>
+        <v>517617</v>
       </c>
       <c r="B60">
-        <v>20150929</v>
+        <v>20150930</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>517612</v>
+        <v>517620</v>
       </c>
       <c r="B61">
-        <v>20151002</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>517617</v>
-      </c>
-      <c r="B62">
-        <v>20150929</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>517617</v>
-      </c>
-      <c r="B63">
-        <v>20150930</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>517620</v>
-      </c>
-      <c r="B64">
         <v>20150930</v>
       </c>
     </row>

</xml_diff>